<commit_message>
修改 riproporre -- ha riproposto
</commit_message>
<xml_diff>
--- a/excel/302 Indicativo - Passato Prossimo.xlsx
+++ b/excel/302 Indicativo - Passato Prossimo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="572">
   <si>
     <t>类别名称</t>
   </si>
@@ -2713,6 +2713,10 @@
   </si>
   <si>
     <t xml:space="preserve"> ha permesso</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ha riproposto</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2821,68 +2825,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3155,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -3168,7 +3111,7 @@
     <col min="5" max="5" width="53.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5943,7 +5886,7 @@
         <v>268</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>503</v>
+        <v>571</v>
       </c>
       <c r="E174" s="5" t="s">
         <v>400</v>

</xml_diff>